<commit_message>
Login medico + atendente
</commit_message>
<xml_diff>
--- a/maissaude/Arquivos/documentações/Diagrama de Classes/Relacionamentos.xlsx
+++ b/maissaude/Arquivos/documentações/Diagrama de Classes/Relacionamentos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro Oliveira\Github\psc\maissaude\Arquivos\documentações\Diagrama de Classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro Oliveira\workspace\Github\psc\maissaude\Arquivos\documentações\Diagrama de Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>1.</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>EstadoReceita</t>
-  </si>
-  <si>
     <t>Medicamento</t>
   </si>
   <si>
@@ -99,6 +96,12 @@
   </si>
   <si>
     <t>Exemplo</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>StatusReceita</t>
   </si>
 </sst>
 </file>
@@ -175,15 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -195,6 +195,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,14 +485,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K10"/>
+  <dimension ref="B3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
@@ -491,38 +501,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -532,43 +542,43 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -582,46 +592,46 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -636,30 +646,64 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>